<commit_message>
Updated product backlog at the start of sprint 2
</commit_message>
<xml_diff>
--- a/Product_Backlog/Agile Product Backlog.xlsx
+++ b/Product_Backlog/Agile Product Backlog.xlsx
@@ -1,27 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danielscheitler\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raufn\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A8DF015-793E-44BE-9905-6EC70D50A388}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-10910" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Product Backlog" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Product Backlog'!$B$2:$M$30</definedName>
-    <definedName name="Priority">'Agile Product Backlog'!$P$5:$P$7</definedName>
-    <definedName name="Status">'Agile Product Backlog'!$Q$5:$Q$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Product Backlog'!$B$2:$M$22</definedName>
+    <definedName name="Priority">'Agile Product Backlog'!$P$5:$P$25</definedName>
+    <definedName name="Status">'Agile Product Backlog'!$Q$5:$Q$25</definedName>
     <definedName name="YesNo">'Agile Product Backlog'!$O$5:$O$6</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -30,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="61">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -62,9 +71,6 @@
     <t>Not Started</t>
   </si>
   <si>
-    <t>TASK ID</t>
-  </si>
-  <si>
     <t>STATUS</t>
   </si>
   <si>
@@ -80,9 +86,6 @@
     <t>SPRINT #</t>
   </si>
   <si>
-    <t>TASK NAME</t>
-  </si>
-  <si>
     <t>STORY</t>
   </si>
   <si>
@@ -98,18 +101,12 @@
     <t>FINISH</t>
   </si>
   <si>
-    <t>" "</t>
-  </si>
-  <si>
     <t>This section is for the drop-down list</t>
   </si>
   <si>
     <t xml:space="preserve">AGILE PRODUCT BACKLOG </t>
   </si>
   <si>
-    <t>User should be able to search procedure by name</t>
-  </si>
-  <si>
     <t>User should be able to search procedure by procedure code</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>User should be able to filter results based on distance</t>
   </si>
   <si>
-    <t>User with account should be able to leave review</t>
-  </si>
-  <si>
     <t>User should be able to access the web application from a mobile phone with a responsive design</t>
   </si>
   <si>
@@ -185,14 +179,56 @@
     <t>Users should be able to to provide their location automatically</t>
   </si>
   <si>
-    <t>???</t>
+    <t>USERSTORY ID</t>
+  </si>
+  <si>
+    <t>User should be able to access the website through the internet</t>
+  </si>
+  <si>
+    <t>Set up the database</t>
+  </si>
+  <si>
+    <t>Rauf Tarar</t>
+  </si>
+  <si>
+    <t>Populate the database</t>
+  </si>
+  <si>
+    <t>Wireframing</t>
+  </si>
+  <si>
+    <t>As a user should be able to search procedure by name</t>
+  </si>
+  <si>
+    <t>Userstory</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Research on cookies</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>colour-filters</t>
+  </si>
+  <si>
+    <t>No one</t>
+  </si>
+  <si>
+    <t>User should be able to leave review</t>
+  </si>
+  <si>
+    <t>User shoulf be able to see previous reviews</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -235,19 +271,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="22"/>
-      <color theme="0"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -337,12 +364,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -375,22 +401,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -726,40 +745,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AI69"/>
+  <dimension ref="B1:AI63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.25" style="4" customWidth="1"/>
-    <col min="2" max="2" width="10.75" style="4" customWidth="1"/>
+    <col min="1" max="1" width="3.19921875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.8984375" style="4" customWidth="1"/>
     <col min="3" max="3" width="40" style="4" customWidth="1"/>
-    <col min="4" max="5" width="33.25" style="4" customWidth="1"/>
-    <col min="6" max="7" width="10.75" style="4" customWidth="1"/>
+    <col min="4" max="5" width="33.19921875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.69921875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.59765625" style="4" customWidth="1"/>
     <col min="8" max="8" width="11.5" style="4" customWidth="1"/>
-    <col min="9" max="9" width="13.75" style="4" customWidth="1"/>
-    <col min="10" max="10" width="15.25" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.75" style="4" customWidth="1"/>
-    <col min="12" max="12" width="13.75" style="4" customWidth="1"/>
-    <col min="13" max="13" width="11.25" style="4" customWidth="1"/>
-    <col min="14" max="14" width="3.25" style="4" customWidth="1"/>
-    <col min="15" max="17" width="17.75" style="4" customWidth="1"/>
+    <col min="9" max="9" width="13.69921875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="15.19921875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.69921875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="13.69921875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="11.19921875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="3.19921875" style="4" customWidth="1"/>
+    <col min="15" max="17" width="17.69921875" style="4" customWidth="1"/>
     <col min="18" max="18" width="15" style="4" customWidth="1"/>
-    <col min="19" max="16384" width="10.75" style="4"/>
+    <col min="19" max="16384" width="10.69921875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:35" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:35" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -795,42 +815,42 @@
       <c r="AH1" s="3"/>
       <c r="AI1" s="3"/>
     </row>
-    <row r="2" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -855,7 +875,7 @@
       <c r="AH2" s="3"/>
       <c r="AI2" s="3"/>
     </row>
-    <row r="3" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
@@ -871,8 +891,8 @@
         <v>8</v>
       </c>
       <c r="L3" s="5">
-        <f>SUM(L4:L24)</f>
-        <v>64</v>
+        <f>SUM(L4:L10)</f>
+        <v>46</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="3"/>
@@ -897,30 +917,36 @@
       <c r="AH3" s="3"/>
       <c r="AI3" s="3"/>
     </row>
-    <row r="4" spans="2:35" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:35" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7">
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="8">
+        <v>43859</v>
+      </c>
+      <c r="G4" s="8">
+        <v>43859</v>
+      </c>
       <c r="H4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="L4" s="7">
         <v>5</v>
@@ -930,11 +956,11 @@
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
@@ -953,30 +979,36 @@
       <c r="AH4" s="3"/>
       <c r="AI4" s="3"/>
     </row>
-    <row r="5" spans="2:35" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:35" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7">
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="8">
+        <v>43860</v>
+      </c>
+      <c r="G5" s="8">
+        <v>43860</v>
+      </c>
       <c r="H5" s="7" t="s">
         <v>2</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="L5" s="7">
         <v>4</v>
@@ -985,17 +1017,17 @@
         <v>2</v>
       </c>
       <c r="N5" s="3"/>
-      <c r="O5" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="P5" s="15" t="s">
+      <c r="O5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="Q5" s="15" t="s">
+      <c r="Q5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="R5" s="15" t="s">
-        <v>44</v>
+      <c r="R5" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
@@ -1015,30 +1047,36 @@
       <c r="AH5" s="3"/>
       <c r="AI5" s="3"/>
     </row>
-    <row r="6" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7">
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="8">
+        <v>43860</v>
+      </c>
+      <c r="G6" s="8">
+        <v>43860</v>
+      </c>
       <c r="H6" s="7" t="s">
         <v>2</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="L6" s="7">
         <v>8</v>
@@ -1047,17 +1085,17 @@
         <v>2</v>
       </c>
       <c r="N6" s="3"/>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="P6" s="15" t="s">
+      <c r="P6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="15" t="s">
+      <c r="Q6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="R6" s="15" t="s">
-        <v>45</v>
+      <c r="R6" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
@@ -1077,46 +1115,51 @@
       <c r="AH6" s="3"/>
       <c r="AI6" s="3"/>
     </row>
-    <row r="7" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7">
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="8">
+        <v>43858</v>
+      </c>
       <c r="G7" s="8"/>
       <c r="H7" s="7" t="s">
         <v>2</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="7">
+        <v>10</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="7">
-        <v>8</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N7" s="3"/>
-      <c r="P7" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q7" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="R7" s="15" t="s">
-        <v>46</v>
+      <c r="R7" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
@@ -1136,41 +1179,49 @@
       <c r="AH7" s="3"/>
       <c r="AI7" s="3"/>
     </row>
-    <row r="8" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>5</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="8">
+        <v>43860</v>
+      </c>
+      <c r="G8" s="8">
+        <v>43860</v>
+      </c>
       <c r="H8" s="7" t="s">
         <v>2</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="L8" s="7">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="M8" s="7" t="s">
         <v>2</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
-      <c r="R8" s="15" t="s">
-        <v>47</v>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="14" t="s">
+        <v>43</v>
       </c>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
@@ -1190,43 +1241,49 @@
       <c r="AH8" s="3"/>
       <c r="AI8" s="3"/>
     </row>
-    <row r="9" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>6</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="8">
+        <v>43859</v>
+      </c>
+      <c r="G9" s="8">
+        <v>43859</v>
+      </c>
       <c r="H9" s="7" t="s">
         <v>2</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="L9" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M9" s="7" t="s">
         <v>2</v>
       </c>
       <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
+      <c r="O9" s="10"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
-      <c r="R9" s="15" t="s">
-        <v>48</v>
+      <c r="R9" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
@@ -1246,41 +1303,45 @@
       <c r="AH9" s="3"/>
       <c r="AI9" s="3"/>
     </row>
-    <row r="10" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
         <v>7</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="8">
+        <v>43860</v>
+      </c>
       <c r="G10" s="8"/>
       <c r="H10" s="7" t="s">
         <v>2</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L10" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="M10" s="7" t="s">
         <v>2</v>
       </c>
       <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
+      <c r="O10" s="10"/>
       <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
+      <c r="Q10" s="11"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
@@ -1300,30 +1361,34 @@
       <c r="AH10" s="3"/>
       <c r="AI10" s="3"/>
     </row>
-    <row r="11" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>8</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="8">
+        <v>43860</v>
+      </c>
       <c r="G11" s="8"/>
       <c r="H11" s="7" t="s">
         <v>2</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L11" s="7">
         <v>5</v>
@@ -1333,8 +1398,8 @@
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="11"/>
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
@@ -1354,41 +1419,47 @@
       <c r="AH11" s="3"/>
       <c r="AI11" s="3"/>
     </row>
-    <row r="12" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>9</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="8">
+        <v>43858</v>
+      </c>
+      <c r="G12" s="8">
+        <v>43858</v>
+      </c>
       <c r="H12" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>51</v>
+        <v>7</v>
+      </c>
+      <c r="L12" s="7">
+        <v>1</v>
       </c>
       <c r="M12" s="7" t="s">
         <v>2</v>
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="11"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
@@ -1408,41 +1479,48 @@
       <c r="AH12" s="3"/>
       <c r="AI12" s="3"/>
     </row>
-    <row r="13" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <v>10</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="F13" s="8">
+        <f>$F$7</f>
+        <v>43858</v>
+      </c>
+      <c r="G13" s="8">
+        <v>43860</v>
+      </c>
       <c r="H13" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>4</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>51</v>
+        <v>7</v>
+      </c>
+      <c r="L13" s="7">
+        <v>5</v>
       </c>
       <c r="M13" s="7" t="s">
         <v>2</v>
       </c>
       <c r="N13" s="3"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="11"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
@@ -1462,38 +1540,47 @@
       <c r="AH13" s="3"/>
       <c r="AI13" s="3"/>
     </row>
-    <row r="14" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
         <v>11</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+        <v>51</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="8">
+        <f>$F$7</f>
+        <v>43858</v>
+      </c>
+      <c r="G14" s="8">
+        <v>43860</v>
+      </c>
       <c r="H14" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J14" s="7" t="s">
         <v>5</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>51</v>
+        <v>7</v>
+      </c>
+      <c r="L14" s="7">
+        <v>10</v>
       </c>
       <c r="M14" s="7" t="s">
         <v>2</v>
       </c>
       <c r="N14" s="3"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="10"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
@@ -1514,33 +1601,39 @@
       <c r="AH14" s="3"/>
       <c r="AI14" s="3"/>
     </row>
-    <row r="15" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="7">
         <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="8">
+        <v>43859</v>
+      </c>
+      <c r="G15" s="8">
+        <v>43859</v>
+      </c>
       <c r="H15" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J15" s="7" t="s">
         <v>6</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>51</v>
+        <v>7</v>
+      </c>
+      <c r="L15" s="7">
+        <v>3</v>
       </c>
       <c r="M15" s="7" t="s">
         <v>2</v>
@@ -1548,7 +1641,7 @@
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="10"/>
-      <c r="Q15" s="11"/>
+      <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
@@ -1568,37 +1661,21 @@
       <c r="AH15" s="3"/>
       <c r="AI15" s="3"/>
     </row>
-    <row r="16" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="7">
-        <v>13</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="M16" s="7" t="s">
-        <v>2</v>
-      </c>
+    <row r="16" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -1622,33 +1699,37 @@
       <c r="AH16" s="3"/>
       <c r="AI16" s="3"/>
     </row>
-    <row r="17" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
+        <v>1</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="8">
+        <v>43864</v>
+      </c>
       <c r="G17" s="8"/>
       <c r="H17" s="7" t="s">
         <v>2</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>51</v>
+        <v>8</v>
+      </c>
+      <c r="L17" s="7">
+        <v>5</v>
       </c>
       <c r="M17" s="7" t="s">
         <v>2</v>
@@ -1676,24 +1757,26 @@
       <c r="AH17" s="3"/>
       <c r="AI17" s="3"/>
     </row>
-    <row r="18" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="7">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="7" t="s">
         <v>2</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>6</v>
@@ -1701,8 +1784,8 @@
       <c r="K18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L18" s="7" t="s">
-        <v>51</v>
+      <c r="L18" s="7">
+        <v>6</v>
       </c>
       <c r="M18" s="7" t="s">
         <v>2</v>
@@ -1730,33 +1813,29 @@
       <c r="AH18" s="3"/>
       <c r="AI18" s="3"/>
     </row>
-    <row r="19" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="7">
-        <v>16</v>
-      </c>
+    <row r="19" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="7"/>
+        <v>56</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
-      <c r="H19" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
       <c r="J19" s="7" t="s">
         <v>6</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L19" s="7" t="s">
-        <v>51</v>
+      <c r="L19" s="7">
+        <v>5</v>
       </c>
       <c r="M19" s="7" t="s">
         <v>2</v>
@@ -1784,36 +1863,38 @@
       <c r="AH19" s="3"/>
       <c r="AI19" s="3"/>
     </row>
-    <row r="20" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="7">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="7" t="s">
         <v>2</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L20" s="7" t="s">
-        <v>51</v>
+      <c r="L20" s="7">
+        <v>6</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -1838,36 +1919,38 @@
       <c r="AH20" s="3"/>
       <c r="AI20" s="3"/>
     </row>
-    <row r="21" spans="2:35" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="7">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="7" t="s">
         <v>2</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>9</v>
       </c>
       <c r="L21" s="7">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
@@ -1892,17 +1975,19 @@
       <c r="AH21" s="3"/>
       <c r="AI21" s="3"/>
     </row>
-    <row r="22" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="7">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="7" t="s">
@@ -1912,16 +1997,16 @@
         <v>3</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>9</v>
       </c>
       <c r="L22" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
@@ -1946,17 +2031,19 @@
       <c r="AH22" s="3"/>
       <c r="AI22" s="3"/>
     </row>
-    <row r="23" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="7">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="7" t="s">
@@ -1966,16 +2053,16 @@
         <v>3</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>9</v>
       </c>
       <c r="L23" s="7">
+        <v>4</v>
+      </c>
+      <c r="M23" s="7" t="s">
         <v>3</v>
-      </c>
-      <c r="M23" s="7" t="s">
-        <v>2</v>
       </c>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
@@ -2000,17 +2087,19 @@
       <c r="AH23" s="3"/>
       <c r="AI23" s="3"/>
     </row>
-    <row r="24" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:35" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="7" t="s">
@@ -2020,16 +2109,16 @@
         <v>3</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L24" s="7" t="s">
-        <v>51</v>
+      <c r="L24" s="7">
+        <v>5</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
@@ -2054,21 +2143,39 @@
       <c r="AH24" s="3"/>
       <c r="AI24" s="3"/>
     </row>
-    <row r="25" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5" t="s">
+    <row r="25" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="7">
+        <v>8</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
+      <c r="E25" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L25" s="7">
+        <v>3</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
@@ -2092,19 +2199,39 @@
       <c r="AH25" s="3"/>
       <c r="AI25" s="3"/>
     </row>
-    <row r="26" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+    <row r="26" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="7">
+        <v>9</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
+      <c r="H26" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L26" s="7">
+        <v>4</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
@@ -2122,25 +2249,40 @@
       <c r="AB26" s="3"/>
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
-      <c r="AE26" s="3"/>
-      <c r="AF26" s="3"/>
-      <c r="AG26" s="3"/>
-      <c r="AH26" s="3"/>
-      <c r="AI26" s="3"/>
-    </row>
-    <row r="27" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
+    </row>
+    <row r="27" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="7">
+        <v>10</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
+      <c r="H27" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L27" s="7">
+        <v>10</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
@@ -2158,25 +2300,40 @@
       <c r="AB27" s="3"/>
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
-      <c r="AE27" s="3"/>
-      <c r="AF27" s="3"/>
-      <c r="AG27" s="3"/>
-      <c r="AH27" s="3"/>
-      <c r="AI27" s="3"/>
-    </row>
-    <row r="28" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
+    </row>
+    <row r="28" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="7">
+        <v>11</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
+      <c r="H28" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L28" s="7">
+        <v>5</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
@@ -2194,25 +2351,40 @@
       <c r="AB28" s="3"/>
       <c r="AC28" s="3"/>
       <c r="AD28" s="3"/>
-      <c r="AE28" s="3"/>
-      <c r="AF28" s="3"/>
-      <c r="AG28" s="3"/>
-      <c r="AH28" s="3"/>
-      <c r="AI28" s="3"/>
-    </row>
-    <row r="29" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
+    </row>
+    <row r="29" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="7">
+        <v>12</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
+      <c r="H29" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L29" s="7">
+        <v>5</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
@@ -2230,25 +2402,40 @@
       <c r="AB29" s="3"/>
       <c r="AC29" s="3"/>
       <c r="AD29" s="3"/>
-      <c r="AE29" s="3"/>
-      <c r="AF29" s="3"/>
-      <c r="AG29" s="3"/>
-      <c r="AH29" s="3"/>
-      <c r="AI29" s="3"/>
-    </row>
-    <row r="30" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
+    </row>
+    <row r="30" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="7">
+        <v>13</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
+      <c r="H30" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L30" s="7">
+        <v>6</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
@@ -2266,24 +2453,40 @@
       <c r="AB30" s="3"/>
       <c r="AC30" s="3"/>
       <c r="AD30" s="3"/>
-      <c r="AE30" s="3"/>
-      <c r="AF30" s="3"/>
-      <c r="AG30" s="3"/>
-      <c r="AH30" s="3"/>
-      <c r="AI30" s="3"/>
-    </row>
-    <row r="31" spans="2:35" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
+    </row>
+    <row r="31" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="7">
+        <v>14</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L31" s="7">
+        <v>6</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
@@ -2301,49 +2504,59 @@
       <c r="AB31" s="3"/>
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
-      <c r="AE31" s="3"/>
-      <c r="AF31" s="3"/>
-      <c r="AG31" s="3"/>
-      <c r="AH31" s="3"/>
-      <c r="AI31" s="3"/>
-    </row>
-    <row r="32" spans="2:35" s="12" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="16"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="10"/>
+    </row>
+    <row r="32" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="7">
+        <v>15</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L32" s="7">
+        <v>3</v>
+      </c>
+      <c r="M32" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N32" s="3"/>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
-      <c r="R32" s="11"/>
-      <c r="S32" s="11"/>
-      <c r="T32" s="11"/>
-      <c r="U32" s="11"/>
-      <c r="V32" s="11"/>
-      <c r="W32" s="11"/>
-      <c r="X32" s="11"/>
-      <c r="Y32" s="11"/>
-      <c r="Z32" s="11"/>
-      <c r="AA32" s="11"/>
-      <c r="AB32" s="11"/>
-      <c r="AC32" s="11"/>
-      <c r="AD32" s="11"/>
-      <c r="AE32" s="11"/>
-      <c r="AF32" s="11"/>
-      <c r="AG32" s="11"/>
-      <c r="AH32" s="11"/>
-      <c r="AI32" s="11"/>
-    </row>
-    <row r="33" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3"/>
+      <c r="AC32" s="3"/>
+      <c r="AD32" s="3"/>
+    </row>
+    <row r="33" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -2378,7 +2591,7 @@
       <c r="AH33" s="3"/>
       <c r="AI33" s="3"/>
     </row>
-    <row r="34" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
@@ -2413,7 +2626,7 @@
       <c r="AH34" s="3"/>
       <c r="AI34" s="3"/>
     </row>
-    <row r="35" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -2448,7 +2661,7 @@
       <c r="AH35" s="3"/>
       <c r="AI35" s="3"/>
     </row>
-    <row r="36" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
@@ -2483,7 +2696,7 @@
       <c r="AH36" s="3"/>
       <c r="AI36" s="3"/>
     </row>
-    <row r="37" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -2518,7 +2731,7 @@
       <c r="AH37" s="3"/>
       <c r="AI37" s="3"/>
     </row>
-    <row r="38" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -2553,7 +2766,7 @@
       <c r="AH38" s="3"/>
       <c r="AI38" s="3"/>
     </row>
-    <row r="39" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -2588,7 +2801,7 @@
       <c r="AH39" s="3"/>
       <c r="AI39" s="3"/>
     </row>
-    <row r="40" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -2623,7 +2836,7 @@
       <c r="AH40" s="3"/>
       <c r="AI40" s="3"/>
     </row>
-    <row r="41" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
@@ -2658,7 +2871,7 @@
       <c r="AH41" s="3"/>
       <c r="AI41" s="3"/>
     </row>
-    <row r="42" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -2693,7 +2906,7 @@
       <c r="AH42" s="3"/>
       <c r="AI42" s="3"/>
     </row>
-    <row r="43" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
@@ -2728,7 +2941,7 @@
       <c r="AH43" s="3"/>
       <c r="AI43" s="3"/>
     </row>
-    <row r="44" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -2763,7 +2976,7 @@
       <c r="AH44" s="3"/>
       <c r="AI44" s="3"/>
     </row>
-    <row r="45" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
@@ -2798,7 +3011,7 @@
       <c r="AH45" s="3"/>
       <c r="AI45" s="3"/>
     </row>
-    <row r="46" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
@@ -2833,7 +3046,7 @@
       <c r="AH46" s="3"/>
       <c r="AI46" s="3"/>
     </row>
-    <row r="47" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
@@ -2868,7 +3081,7 @@
       <c r="AH47" s="3"/>
       <c r="AI47" s="3"/>
     </row>
-    <row r="48" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -2903,7 +3116,7 @@
       <c r="AH48" s="3"/>
       <c r="AI48" s="3"/>
     </row>
-    <row r="49" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
@@ -2938,7 +3151,7 @@
       <c r="AH49" s="3"/>
       <c r="AI49" s="3"/>
     </row>
-    <row r="50" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -2951,9 +3164,7 @@
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
-      <c r="O50" s="3"/>
       <c r="P50" s="3"/>
-      <c r="Q50" s="3"/>
       <c r="R50" s="3"/>
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
@@ -2973,7 +3184,7 @@
       <c r="AH50" s="3"/>
       <c r="AI50" s="3"/>
     </row>
-    <row r="51" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
@@ -2986,9 +3197,6 @@
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
       <c r="T51" s="3"/>
@@ -3008,7 +3216,7 @@
       <c r="AH51" s="3"/>
       <c r="AI51" s="3"/>
     </row>
-    <row r="52" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
@@ -3021,9 +3229,6 @@
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
-      <c r="P52" s="3"/>
-      <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
       <c r="S52" s="3"/>
       <c r="T52" s="3"/>
@@ -3043,7 +3248,7 @@
       <c r="AH52" s="3"/>
       <c r="AI52" s="3"/>
     </row>
-    <row r="53" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -3056,9 +3261,6 @@
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
       <c r="N53" s="3"/>
-      <c r="O53" s="3"/>
-      <c r="P53" s="3"/>
-      <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
       <c r="S53" s="3"/>
       <c r="T53" s="3"/>
@@ -3078,7 +3280,7 @@
       <c r="AH53" s="3"/>
       <c r="AI53" s="3"/>
     </row>
-    <row r="54" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
@@ -3091,9 +3293,6 @@
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
       <c r="N54" s="3"/>
-      <c r="O54" s="3"/>
-      <c r="P54" s="3"/>
-      <c r="Q54" s="3"/>
       <c r="R54" s="3"/>
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
@@ -3113,7 +3312,7 @@
       <c r="AH54" s="3"/>
       <c r="AI54" s="3"/>
     </row>
-    <row r="55" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -3126,9 +3325,6 @@
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
       <c r="N55" s="3"/>
-      <c r="O55" s="3"/>
-      <c r="P55" s="3"/>
-      <c r="Q55" s="3"/>
       <c r="R55" s="3"/>
       <c r="S55" s="3"/>
       <c r="T55" s="3"/>
@@ -3148,7 +3344,7 @@
       <c r="AH55" s="3"/>
       <c r="AI55" s="3"/>
     </row>
-    <row r="56" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
@@ -3161,9 +3357,6 @@
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
       <c r="N56" s="3"/>
-      <c r="O56" s="3"/>
-      <c r="P56" s="3"/>
-      <c r="Q56" s="3"/>
       <c r="R56" s="3"/>
       <c r="S56" s="3"/>
       <c r="T56" s="3"/>
@@ -3183,7 +3376,7 @@
       <c r="AH56" s="3"/>
       <c r="AI56" s="3"/>
     </row>
-    <row r="57" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
@@ -3196,8 +3389,6 @@
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
       <c r="N57" s="3"/>
-      <c r="P57" s="3"/>
-      <c r="Q57" s="3"/>
       <c r="R57" s="3"/>
       <c r="S57" s="3"/>
       <c r="T57" s="3"/>
@@ -3217,7 +3408,7 @@
       <c r="AH57" s="3"/>
       <c r="AI57" s="3"/>
     </row>
-    <row r="58" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
@@ -3249,7 +3440,7 @@
       <c r="AH58" s="3"/>
       <c r="AI58" s="3"/>
     </row>
-    <row r="59" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -3281,7 +3472,7 @@
       <c r="AH59" s="3"/>
       <c r="AI59" s="3"/>
     </row>
-    <row r="60" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -3313,7 +3504,7 @@
       <c r="AH60" s="3"/>
       <c r="AI60" s="3"/>
     </row>
-    <row r="61" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -3345,7 +3536,7 @@
       <c r="AH61" s="3"/>
       <c r="AI61" s="3"/>
     </row>
-    <row r="62" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -3377,21 +3568,8 @@
       <c r="AH62" s="3"/>
       <c r="AI62" s="3"/>
     </row>
-    <row r="63" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
-      <c r="J63" s="3"/>
-      <c r="K63" s="3"/>
-      <c r="L63" s="3"/>
-      <c r="M63" s="3"/>
+    <row r="63" spans="3:35" x14ac:dyDescent="0.3">
       <c r="N63" s="3"/>
-      <c r="R63" s="3"/>
-      <c r="S63" s="3"/>
       <c r="T63" s="3"/>
       <c r="U63" s="3"/>
       <c r="V63" s="3"/>
@@ -3409,218 +3587,24 @@
       <c r="AH63" s="3"/>
       <c r="AI63" s="3"/>
     </row>
-    <row r="64" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
-      <c r="J64" s="3"/>
-      <c r="K64" s="3"/>
-      <c r="L64" s="3"/>
-      <c r="M64" s="3"/>
-      <c r="N64" s="3"/>
-      <c r="R64" s="3"/>
-      <c r="S64" s="3"/>
-      <c r="T64" s="3"/>
-      <c r="U64" s="3"/>
-      <c r="V64" s="3"/>
-      <c r="W64" s="3"/>
-      <c r="X64" s="3"/>
-      <c r="Y64" s="3"/>
-      <c r="Z64" s="3"/>
-      <c r="AA64" s="3"/>
-      <c r="AB64" s="3"/>
-      <c r="AC64" s="3"/>
-      <c r="AD64" s="3"/>
-      <c r="AE64" s="3"/>
-      <c r="AF64" s="3"/>
-      <c r="AG64" s="3"/>
-      <c r="AH64" s="3"/>
-      <c r="AI64" s="3"/>
-    </row>
-    <row r="65" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
-      <c r="J65" s="3"/>
-      <c r="K65" s="3"/>
-      <c r="L65" s="3"/>
-      <c r="M65" s="3"/>
-      <c r="N65" s="3"/>
-      <c r="R65" s="3"/>
-      <c r="S65" s="3"/>
-      <c r="T65" s="3"/>
-      <c r="U65" s="3"/>
-      <c r="V65" s="3"/>
-      <c r="W65" s="3"/>
-      <c r="X65" s="3"/>
-      <c r="Y65" s="3"/>
-      <c r="Z65" s="3"/>
-      <c r="AA65" s="3"/>
-      <c r="AB65" s="3"/>
-      <c r="AC65" s="3"/>
-      <c r="AD65" s="3"/>
-      <c r="AE65" s="3"/>
-      <c r="AF65" s="3"/>
-      <c r="AG65" s="3"/>
-      <c r="AH65" s="3"/>
-      <c r="AI65" s="3"/>
-    </row>
-    <row r="66" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
-      <c r="J66" s="3"/>
-      <c r="K66" s="3"/>
-      <c r="L66" s="3"/>
-      <c r="M66" s="3"/>
-      <c r="N66" s="3"/>
-      <c r="R66" s="3"/>
-      <c r="S66" s="3"/>
-      <c r="T66" s="3"/>
-      <c r="U66" s="3"/>
-      <c r="V66" s="3"/>
-      <c r="W66" s="3"/>
-      <c r="X66" s="3"/>
-      <c r="Y66" s="3"/>
-      <c r="Z66" s="3"/>
-      <c r="AA66" s="3"/>
-      <c r="AB66" s="3"/>
-      <c r="AC66" s="3"/>
-      <c r="AD66" s="3"/>
-      <c r="AE66" s="3"/>
-      <c r="AF66" s="3"/>
-      <c r="AG66" s="3"/>
-      <c r="AH66" s="3"/>
-      <c r="AI66" s="3"/>
-    </row>
-    <row r="67" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
-      <c r="J67" s="3"/>
-      <c r="K67" s="3"/>
-      <c r="L67" s="3"/>
-      <c r="M67" s="3"/>
-      <c r="N67" s="3"/>
-      <c r="R67" s="3"/>
-      <c r="S67" s="3"/>
-      <c r="T67" s="3"/>
-      <c r="U67" s="3"/>
-      <c r="V67" s="3"/>
-      <c r="W67" s="3"/>
-      <c r="X67" s="3"/>
-      <c r="Y67" s="3"/>
-      <c r="Z67" s="3"/>
-      <c r="AA67" s="3"/>
-      <c r="AB67" s="3"/>
-      <c r="AC67" s="3"/>
-      <c r="AD67" s="3"/>
-      <c r="AE67" s="3"/>
-      <c r="AF67" s="3"/>
-      <c r="AG67" s="3"/>
-      <c r="AH67" s="3"/>
-      <c r="AI67" s="3"/>
-    </row>
-    <row r="68" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
-      <c r="J68" s="3"/>
-      <c r="K68" s="3"/>
-      <c r="L68" s="3"/>
-      <c r="M68" s="3"/>
-      <c r="N68" s="3"/>
-      <c r="R68" s="3"/>
-      <c r="S68" s="3"/>
-      <c r="T68" s="3"/>
-      <c r="U68" s="3"/>
-      <c r="V68" s="3"/>
-      <c r="W68" s="3"/>
-      <c r="X68" s="3"/>
-      <c r="Y68" s="3"/>
-      <c r="Z68" s="3"/>
-      <c r="AA68" s="3"/>
-      <c r="AB68" s="3"/>
-      <c r="AC68" s="3"/>
-      <c r="AD68" s="3"/>
-      <c r="AE68" s="3"/>
-      <c r="AF68" s="3"/>
-      <c r="AG68" s="3"/>
-      <c r="AH68" s="3"/>
-      <c r="AI68" s="3"/>
-    </row>
-    <row r="69" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
-      <c r="H69" s="3"/>
-      <c r="I69" s="3"/>
-      <c r="J69" s="3"/>
-      <c r="K69" s="3"/>
-      <c r="L69" s="3"/>
-      <c r="M69" s="3"/>
-      <c r="N69" s="3"/>
-      <c r="R69" s="3"/>
-      <c r="S69" s="3"/>
-      <c r="T69" s="3"/>
-      <c r="U69" s="3"/>
-      <c r="V69" s="3"/>
-      <c r="W69" s="3"/>
-      <c r="X69" s="3"/>
-      <c r="Y69" s="3"/>
-      <c r="Z69" s="3"/>
-      <c r="AA69" s="3"/>
-      <c r="AB69" s="3"/>
-      <c r="AC69" s="3"/>
-      <c r="AD69" s="3"/>
-      <c r="AE69" s="3"/>
-      <c r="AF69" s="3"/>
-      <c r="AG69" s="3"/>
-      <c r="AH69" s="3"/>
-      <c r="AI69" s="3"/>
-    </row>
   </sheetData>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:I30 M3:M30">
+  <phoneticPr fontId="6" type="noConversion"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:I32 M3:M32" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>YesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J32" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>Priority</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K32" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>Status</formula1>
     </dataValidation>
-    <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O6">
-      <formula1>$A$6:$A$25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E24">
-      <formula1>$R$5:$R$9</formula1>
+    <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O6" xr:uid="{00000000-0002-0000-0000-000003000000}">
+      <formula1>$A$6:$A$17</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
-  <pageSetup scale="58" fitToHeight="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="58" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated Sprint and product backlog
</commit_message>
<xml_diff>
--- a/Product_Backlog/Agile Product Backlog.xlsx
+++ b/Product_Backlog/Agile Product Backlog.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raufn\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A8DF015-793E-44BE-9905-6EC70D50A388}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CC9183-87B6-4A3E-8623-83DC25273759}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-10910" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Product Backlog" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Product Backlog'!$B$2:$M$22</definedName>
-    <definedName name="Priority">'Agile Product Backlog'!$P$5:$P$25</definedName>
-    <definedName name="Status">'Agile Product Backlog'!$Q$5:$Q$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Product Backlog'!$B$2:$M$23</definedName>
+    <definedName name="Priority">'Agile Product Backlog'!$P$5:$P$26</definedName>
+    <definedName name="Status">'Agile Product Backlog'!$Q$5:$Q$26</definedName>
     <definedName name="YesNo">'Agile Product Backlog'!$O$5:$O$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="61">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -750,11 +750,11 @@
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AI63"/>
+  <dimension ref="B1:AI62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
@@ -891,8 +891,8 @@
         <v>8</v>
       </c>
       <c r="L3" s="5">
-        <f>SUM(L4:L10)</f>
-        <v>46</v>
+        <f>SUM(L4:L18)</f>
+        <v>90</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="3"/>
@@ -1115,12 +1115,12 @@
       <c r="AH6" s="3"/>
       <c r="AI6" s="3"/>
     </row>
-    <row r="7" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>0</v>
@@ -1129,7 +1129,7 @@
         <v>39</v>
       </c>
       <c r="F7" s="8">
-        <v>43858</v>
+        <v>43860</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="7" t="s">
@@ -1139,28 +1139,22 @@
         <v>2</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>8</v>
       </c>
       <c r="L7" s="7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="M7" s="7" t="s">
         <v>2</v>
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
-      <c r="P7" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q7" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="R7" s="14" t="s">
-        <v>42</v>
-      </c>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="3"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
@@ -1179,50 +1173,48 @@
       <c r="AH7" s="3"/>
       <c r="AI7" s="3"/>
     </row>
-    <row r="8" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F8" s="8">
-        <v>43860</v>
+        <v>43858</v>
       </c>
       <c r="G8" s="8">
-        <v>43860</v>
+        <v>43858</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>2</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="L8" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M8" s="7" t="s">
         <v>2</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="14" t="s">
-        <v>43</v>
-      </c>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="3"/>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
@@ -1241,50 +1233,49 @@
       <c r="AH8" s="3"/>
       <c r="AI8" s="3"/>
     </row>
-    <row r="9" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="F9" s="8">
-        <v>43859</v>
+        <f>$F$17</f>
+        <v>43858</v>
       </c>
       <c r="G9" s="8">
-        <v>43859</v>
+        <v>43860</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>2</v>
       </c>
       <c r="J9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="7">
         <v>5</v>
       </c>
-      <c r="K9" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="L9" s="7">
-        <v>4</v>
-      </c>
       <c r="M9" s="7" t="s">
         <v>2</v>
       </c>
       <c r="N9" s="3"/>
-      <c r="O9" s="10"/>
+      <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
-      <c r="R9" s="14" t="s">
-        <v>41</v>
-      </c>
+      <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
@@ -1298,28 +1289,26 @@
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
       <c r="AE9" s="3"/>
-      <c r="AF9" s="3"/>
-      <c r="AG9" s="3"/>
-      <c r="AH9" s="3"/>
-      <c r="AI9" s="3"/>
     </row>
     <row r="10" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F10" s="8">
         <v>43860</v>
       </c>
-      <c r="G10" s="8"/>
+      <c r="G10" s="8">
+        <v>43860</v>
+      </c>
       <c r="H10" s="7" t="s">
         <v>2</v>
       </c>
@@ -1327,21 +1316,21 @@
         <v>2</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="L10" s="7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="M10" s="7" t="s">
         <v>2</v>
       </c>
       <c r="N10" s="3"/>
-      <c r="O10" s="10"/>
+      <c r="O10" s="3"/>
       <c r="P10" s="3"/>
-      <c r="Q10" s="11"/>
+      <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
@@ -1356,17 +1345,13 @@
       <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
       <c r="AE10" s="3"/>
-      <c r="AF10" s="3"/>
-      <c r="AG10" s="3"/>
-      <c r="AH10" s="3"/>
-      <c r="AI10" s="3"/>
-    </row>
-    <row r="11" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>0</v>
@@ -1375,9 +1360,11 @@
         <v>39</v>
       </c>
       <c r="F11" s="8">
-        <v>43860</v>
-      </c>
-      <c r="G11" s="8"/>
+        <v>43859</v>
+      </c>
+      <c r="G11" s="8">
+        <v>43859</v>
+      </c>
       <c r="H11" s="7" t="s">
         <v>2</v>
       </c>
@@ -1385,21 +1372,21 @@
         <v>2</v>
       </c>
       <c r="J11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="L11" s="7">
         <v>4</v>
       </c>
-      <c r="K11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="L11" s="7">
-        <v>5</v>
-      </c>
       <c r="M11" s="7" t="s">
         <v>2</v>
       </c>
       <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="11"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
@@ -1414,29 +1401,26 @@
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
       <c r="AE11" s="3"/>
-      <c r="AF11" s="3"/>
-      <c r="AG11" s="3"/>
-      <c r="AH11" s="3"/>
-      <c r="AI11" s="3"/>
     </row>
     <row r="12" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F12" s="8">
+        <f>$F$17</f>
         <v>43858</v>
       </c>
       <c r="G12" s="8">
-        <v>43858</v>
+        <v>43860</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>3</v>
@@ -1445,21 +1429,21 @@
         <v>2</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>7</v>
       </c>
       <c r="L12" s="7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="M12" s="7" t="s">
         <v>2</v>
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="11"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
@@ -1474,42 +1458,35 @@
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
       <c r="AE12" s="3"/>
-      <c r="AF12" s="3"/>
-      <c r="AG12" s="3"/>
-      <c r="AH12" s="3"/>
-      <c r="AI12" s="3"/>
-    </row>
-    <row r="13" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>49</v>
+        <v>1</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="F13" s="8">
-        <f>$F$7</f>
-        <v>43858</v>
-      </c>
-      <c r="G13" s="8">
-        <v>43860</v>
-      </c>
+        <v>43866</v>
+      </c>
+      <c r="G13" s="8"/>
       <c r="H13" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>2</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L13" s="7">
         <v>5</v>
@@ -1519,8 +1496,8 @@
       </c>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="11"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
@@ -1530,38 +1507,26 @@
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
-      <c r="AA13" s="3"/>
-      <c r="AB13" s="3"/>
-      <c r="AC13" s="3"/>
-      <c r="AD13" s="3"/>
-      <c r="AE13" s="3"/>
-      <c r="AF13" s="3"/>
-      <c r="AG13" s="3"/>
-      <c r="AH13" s="3"/>
-      <c r="AI13" s="3"/>
-    </row>
-    <row r="14" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>41</v>
       </c>
       <c r="F14" s="8">
-        <f>$F$7</f>
-        <v>43858</v>
-      </c>
-      <c r="G14" s="8">
-        <v>43860</v>
-      </c>
+        <v>43864</v>
+      </c>
+      <c r="G14" s="8"/>
       <c r="H14" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>2</v>
@@ -1570,17 +1535,17 @@
         <v>5</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L14" s="7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="M14" s="7" t="s">
         <v>2</v>
       </c>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
-      <c r="P14" s="10"/>
+      <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
@@ -1596,51 +1561,45 @@
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
       <c r="AE14" s="3"/>
-      <c r="AF14" s="3"/>
-      <c r="AG14" s="3"/>
-      <c r="AH14" s="3"/>
-      <c r="AI14" s="3"/>
-    </row>
-    <row r="15" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="7">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>42</v>
+        <v>1</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="F15" s="8">
-        <v>43859</v>
-      </c>
-      <c r="G15" s="8">
-        <v>43859</v>
-      </c>
+        <v>43866</v>
+      </c>
+      <c r="G15" s="8"/>
       <c r="H15" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>2</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L15" s="7">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="M15" s="7" t="s">
         <v>2</v>
       </c>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
-      <c r="P15" s="10"/>
+      <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
@@ -1651,31 +1610,44 @@
       <c r="X15" s="3"/>
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
-      <c r="AA15" s="3"/>
-      <c r="AB15" s="3"/>
-      <c r="AC15" s="3"/>
-      <c r="AD15" s="3"/>
-      <c r="AE15" s="3"/>
-      <c r="AF15" s="3"/>
-      <c r="AG15" s="3"/>
-      <c r="AH15" s="3"/>
-      <c r="AI15" s="3"/>
-    </row>
-    <row r="16" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
+    </row>
+    <row r="16" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="7">
+        <v>12</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="8">
+        <v>43859</v>
+      </c>
+      <c r="G16" s="8">
+        <v>43859</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L16" s="7">
+        <v>3</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -1694,28 +1666,26 @@
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
       <c r="AE16" s="3"/>
-      <c r="AF16" s="3"/>
-      <c r="AG16" s="3"/>
-      <c r="AH16" s="3"/>
-      <c r="AI16" s="3"/>
     </row>
     <row r="17" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>41</v>
+        <v>0</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="F17" s="8">
-        <v>43864</v>
-      </c>
-      <c r="G17" s="8"/>
+        <v>43858</v>
+      </c>
+      <c r="G17" s="8">
+        <v>43867</v>
+      </c>
       <c r="H17" s="7" t="s">
         <v>2</v>
       </c>
@@ -1723,13 +1693,13 @@
         <v>2</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>8</v>
       </c>
       <c r="L17" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="M17" s="7" t="s">
         <v>2</v>
@@ -1752,25 +1722,23 @@
       <c r="AC17" s="3"/>
       <c r="AD17" s="3"/>
       <c r="AE17" s="3"/>
-      <c r="AF17" s="3"/>
-      <c r="AG17" s="3"/>
-      <c r="AH17" s="3"/>
-      <c r="AI17" s="3"/>
     </row>
     <row r="18" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="7">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="8"/>
+      <c r="F18" s="8">
+        <v>43860</v>
+      </c>
       <c r="G18" s="8"/>
       <c r="H18" s="7" t="s">
         <v>2</v>
@@ -1782,16 +1750,16 @@
         <v>6</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L18" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="M18" s="7" t="s">
         <v>2</v>
       </c>
       <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
+      <c r="O18" s="10"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
@@ -1808,26 +1776,28 @@
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
       <c r="AE18" s="3"/>
-      <c r="AF18" s="3"/>
-      <c r="AG18" s="3"/>
-      <c r="AH18" s="3"/>
-      <c r="AI18" s="3"/>
     </row>
     <row r="19" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="7"/>
+      <c r="B19" s="7">
+        <v>2</v>
+      </c>
       <c r="C19" s="7" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>41</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="H19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="J19" s="7" t="s">
         <v>6</v>
       </c>
@@ -1835,7 +1805,7 @@
         <v>9</v>
       </c>
       <c r="L19" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M19" s="7" t="s">
         <v>2</v>
@@ -1864,26 +1834,20 @@
       <c r="AI19" s="3"/>
     </row>
     <row r="20" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="7">
-        <v>3</v>
-      </c>
+      <c r="B20" s="7"/>
       <c r="C20" s="7" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
-      <c r="H20" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
       <c r="J20" s="7" t="s">
         <v>6</v>
       </c>
@@ -1891,10 +1855,10 @@
         <v>9</v>
       </c>
       <c r="L20" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -1921,10 +1885,10 @@
     </row>
     <row r="21" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>1</v>
@@ -1947,7 +1911,7 @@
         <v>9</v>
       </c>
       <c r="L21" s="7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M21" s="7" t="s">
         <v>3</v>
@@ -1977,10 +1941,10 @@
     </row>
     <row r="22" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>1</v>
@@ -1994,7 +1958,7 @@
         <v>2</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>6</v>
@@ -2003,7 +1967,7 @@
         <v>9</v>
       </c>
       <c r="L22" s="7">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="M22" s="7" t="s">
         <v>3</v>
@@ -2033,10 +1997,10 @@
     </row>
     <row r="23" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>1</v>
@@ -2059,7 +2023,7 @@
         <v>9</v>
       </c>
       <c r="L23" s="7">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="M23" s="7" t="s">
         <v>3</v>
@@ -2087,12 +2051,12 @@
       <c r="AH23" s="3"/>
       <c r="AI23" s="3"/>
     </row>
-    <row r="24" spans="2:35" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>1</v>
@@ -2115,7 +2079,7 @@
         <v>9</v>
       </c>
       <c r="L24" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M24" s="7" t="s">
         <v>3</v>
@@ -2143,12 +2107,12 @@
       <c r="AH24" s="3"/>
       <c r="AI24" s="3"/>
     </row>
-    <row r="25" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:35" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>1</v>
@@ -2171,7 +2135,7 @@
         <v>9</v>
       </c>
       <c r="L25" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M25" s="7" t="s">
         <v>3</v>
@@ -2201,10 +2165,10 @@
     </row>
     <row r="26" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>1</v>
@@ -2218,7 +2182,7 @@
         <v>2</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J26" s="7" t="s">
         <v>6</v>
@@ -2227,7 +2191,7 @@
         <v>9</v>
       </c>
       <c r="L26" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M26" s="7" t="s">
         <v>3</v>
@@ -2249,19 +2213,24 @@
       <c r="AB26" s="3"/>
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="3"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
     </row>
     <row r="27" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
@@ -2272,16 +2241,16 @@
         <v>2</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>9</v>
       </c>
       <c r="L27" s="7">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
@@ -2354,16 +2323,16 @@
     </row>
     <row r="29" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
@@ -2374,16 +2343,16 @@
         <v>2</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K29" s="7" t="s">
         <v>9</v>
       </c>
       <c r="L29" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
@@ -2405,16 +2374,16 @@
     </row>
     <row r="30" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="7">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E30" s="8" t="s">
-        <v>58</v>
+      <c r="E30" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
@@ -2434,7 +2403,7 @@
         <v>6</v>
       </c>
       <c r="M30" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
@@ -2456,16 +2425,16 @@
     </row>
     <row r="31" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="7">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>43</v>
+      <c r="E31" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
@@ -2482,7 +2451,7 @@
         <v>9</v>
       </c>
       <c r="L31" s="7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M31" s="7" t="s">
         <v>2</v>
@@ -2505,39 +2474,18 @@
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
     </row>
-    <row r="32" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="7">
-        <v>15</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J32" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="K32" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L32" s="7">
-        <v>3</v>
-      </c>
-      <c r="M32" s="7" t="s">
-        <v>2</v>
-      </c>
+    <row r="32" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
@@ -2555,6 +2503,11 @@
       <c r="AB32" s="3"/>
       <c r="AC32" s="3"/>
       <c r="AD32" s="3"/>
+      <c r="AE32" s="3"/>
+      <c r="AF32" s="3"/>
+      <c r="AG32" s="3"/>
+      <c r="AH32" s="3"/>
+      <c r="AI32" s="3"/>
     </row>
     <row r="33" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C33" s="3"/>
@@ -3129,9 +3082,7 @@
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
-      <c r="O49" s="3"/>
       <c r="P49" s="3"/>
-      <c r="Q49" s="3"/>
       <c r="R49" s="3"/>
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
@@ -3164,7 +3115,6 @@
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
-      <c r="P50" s="3"/>
       <c r="R50" s="3"/>
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
@@ -3537,20 +3487,7 @@
       <c r="AI61" s="3"/>
     </row>
     <row r="62" spans="3:35" x14ac:dyDescent="0.3">
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="3"/>
-      <c r="K62" s="3"/>
-      <c r="L62" s="3"/>
-      <c r="M62" s="3"/>
       <c r="N62" s="3"/>
-      <c r="R62" s="3"/>
-      <c r="S62" s="3"/>
       <c r="T62" s="3"/>
       <c r="U62" s="3"/>
       <c r="V62" s="3"/>
@@ -3568,39 +3505,20 @@
       <c r="AH62" s="3"/>
       <c r="AI62" s="3"/>
     </row>
-    <row r="63" spans="3:35" x14ac:dyDescent="0.3">
-      <c r="N63" s="3"/>
-      <c r="T63" s="3"/>
-      <c r="U63" s="3"/>
-      <c r="V63" s="3"/>
-      <c r="W63" s="3"/>
-      <c r="X63" s="3"/>
-      <c r="Y63" s="3"/>
-      <c r="Z63" s="3"/>
-      <c r="AA63" s="3"/>
-      <c r="AB63" s="3"/>
-      <c r="AC63" s="3"/>
-      <c r="AD63" s="3"/>
-      <c r="AE63" s="3"/>
-      <c r="AF63" s="3"/>
-      <c r="AG63" s="3"/>
-      <c r="AH63" s="3"/>
-      <c r="AI63" s="3"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:I32 M3:M32" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:I6 H7:I31 M3:M6 M7:M31" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>YesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J32" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J6 J7:J31" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>Priority</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K32" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K6 K7:K31" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>Status</formula1>
     </dataValidation>
     <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O6" xr:uid="{00000000-0002-0000-0000-000003000000}">
-      <formula1>$A$6:$A$17</formula1>
+      <formula1>$A$6:$A$14</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>

</xml_diff>

<commit_message>
Updated the product backlog and sprint backlog
</commit_message>
<xml_diff>
--- a/Product_Backlog/Agile Product Backlog.xlsx
+++ b/Product_Backlog/Agile Product Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raufn\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CC9183-87B6-4A3E-8623-83DC25273759}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE9E140-E344-44F5-87FC-EE33FFA0DAD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="60">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -201,9 +201,6 @@
   </si>
   <si>
     <t>Userstory</t>
-  </si>
-  <si>
-    <t>Done</t>
   </si>
   <si>
     <t>Research on cookies</t>
@@ -752,9 +749,9 @@
   </sheetPr>
   <dimension ref="B1:AI62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
@@ -946,7 +943,7 @@
         <v>4</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="L4" s="7">
         <v>5</v>
@@ -1008,7 +1005,7 @@
         <v>4</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="L5" s="7">
         <v>4</v>
@@ -1076,7 +1073,7 @@
         <v>4</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="L6" s="7">
         <v>8</v>
@@ -1117,7 +1114,7 @@
     </row>
     <row r="7" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>47</v>
@@ -1131,7 +1128,9 @@
       <c r="F7" s="8">
         <v>43860</v>
       </c>
-      <c r="G7" s="8"/>
+      <c r="G7" s="8">
+        <v>43868</v>
+      </c>
       <c r="H7" s="7" t="s">
         <v>2</v>
       </c>
@@ -1142,7 +1141,7 @@
         <v>4</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L7" s="7">
         <v>5</v>
@@ -1175,7 +1174,7 @@
     </row>
     <row r="8" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>48</v>
@@ -1235,7 +1234,7 @@
     </row>
     <row r="9" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>50</v>
@@ -1292,7 +1291,7 @@
     </row>
     <row r="10" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>27</v>
@@ -1319,7 +1318,7 @@
         <v>5</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="L10" s="7">
         <v>5</v>
@@ -1348,7 +1347,7 @@
     </row>
     <row r="11" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>45</v>
@@ -1375,7 +1374,7 @@
         <v>5</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="L11" s="7">
         <v>4</v>
@@ -1404,7 +1403,7 @@
     </row>
     <row r="12" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>51</v>
@@ -1461,7 +1460,7 @@
     </row>
     <row r="13" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>28</v>
@@ -1486,7 +1485,7 @@
         <v>5</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L13" s="7">
         <v>5</v>
@@ -1510,7 +1509,7 @@
     </row>
     <row r="14" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>30</v>
@@ -1524,7 +1523,9 @@
       <c r="F14" s="8">
         <v>43864</v>
       </c>
-      <c r="G14" s="8"/>
+      <c r="G14" s="8">
+        <v>43868</v>
+      </c>
       <c r="H14" s="7" t="s">
         <v>2</v>
       </c>
@@ -1535,7 +1536,7 @@
         <v>5</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L14" s="7">
         <v>5</v>
@@ -1564,7 +1565,7 @@
     </row>
     <row r="15" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="7">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>23</v>
@@ -1589,7 +1590,7 @@
         <v>5</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L15" s="7">
         <v>10</v>
@@ -1613,10 +1614,10 @@
     </row>
     <row r="16" spans="2:35" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>0</v>
@@ -1669,7 +1670,7 @@
     </row>
     <row r="17" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>26</v>
@@ -1683,9 +1684,7 @@
       <c r="F17" s="8">
         <v>43858</v>
       </c>
-      <c r="G17" s="8">
-        <v>43867</v>
-      </c>
+      <c r="G17" s="8"/>
       <c r="H17" s="7" t="s">
         <v>2</v>
       </c>
@@ -1725,7 +1724,7 @@
     </row>
     <row r="18" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="7">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>29</v>
@@ -1739,7 +1738,9 @@
       <c r="F18" s="8">
         <v>43860</v>
       </c>
-      <c r="G18" s="8"/>
+      <c r="G18" s="8">
+        <v>43867</v>
+      </c>
       <c r="H18" s="7" t="s">
         <v>2</v>
       </c>
@@ -1750,7 +1751,7 @@
         <v>6</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L18" s="7">
         <v>10</v>
@@ -1779,7 +1780,7 @@
     </row>
     <row r="19" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="7">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>31</v>
@@ -1834,20 +1835,30 @@
       <c r="AI19" s="3"/>
     </row>
     <row r="20" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="7"/>
+      <c r="B20" s="7">
+        <v>17</v>
+      </c>
       <c r="C20" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="F20" s="8">
+        <v>43867</v>
+      </c>
+      <c r="G20" s="8">
+        <v>43867</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="J20" s="7" t="s">
         <v>6</v>
       </c>
@@ -1885,16 +1896,16 @@
     </row>
     <row r="21" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="7">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
@@ -1941,16 +1952,16 @@
     </row>
     <row r="22" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="7">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
@@ -1997,16 +2008,16 @@
     </row>
     <row r="23" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="7">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
@@ -2053,16 +2064,16 @@
     </row>
     <row r="24" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
@@ -2109,16 +2120,16 @@
     </row>
     <row r="25" spans="2:35" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
@@ -2165,16 +2176,16 @@
     </row>
     <row r="26" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
@@ -2221,16 +2232,16 @@
     </row>
     <row r="27" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="7">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>38</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
@@ -2272,16 +2283,16 @@
     </row>
     <row r="28" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="7">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
@@ -2323,16 +2334,16 @@
     </row>
     <row r="29" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="7">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
@@ -2374,13 +2385,13 @@
     </row>
     <row r="30" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="7">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>43</v>
@@ -2425,13 +2436,13 @@
     </row>
     <row r="31" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="7">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>44</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>39</v>
@@ -3508,13 +3519,13 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:I6 H7:I31 M3:M6 M7:M31" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:I31 M3:M31" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>YesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J6 J7:J31" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J31" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>Priority</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K6 K7:K31" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K31" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>Status</formula1>
     </dataValidation>
     <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O6" xr:uid="{00000000-0002-0000-0000-000003000000}">

</xml_diff>